<commit_message>
(^) import nilai method
</commit_message>
<xml_diff>
--- a/resources/assets/imports/import.xlsx
+++ b/resources/assets/imports/import.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="293">
   <si>
     <t>IMPOR NILAI</t>
   </si>
@@ -22,7 +22,7 @@
     <t>KKN TIM I 2022/2023 UNIVERSITAS DIPONEGORO</t>
   </si>
   <si>
-    <t>KECAMATAN Wanasari</t>
+    <t>KECAMATAN Bulakamba</t>
   </si>
   <si>
     <t>KABUPATEN Brebes</t>
@@ -91,16 +91,16 @@
     <t>Format SIAP</t>
   </si>
   <si>
-    <t>12010119130162</t>
-  </si>
-  <si>
-    <t>A. ZAINUL MAJIED NOOR</t>
+    <t>12010118190171</t>
+  </si>
+  <si>
+    <t>AHMAD ARIF NUGROHO</t>
   </si>
   <si>
     <t>Laki-laki</t>
   </si>
   <si>
-    <t>82348395858</t>
+    <t>81584222665</t>
   </si>
   <si>
     <t>Manajemen</t>
@@ -109,208 +109,199 @@
     <t>Fakultas Ekonomika dan Bisnis</t>
   </si>
   <si>
-    <t>12020119140178</t>
-  </si>
-  <si>
-    <t>Adsel Anselmus</t>
-  </si>
-  <si>
-    <t>82243516643</t>
+    <t>12010119190243</t>
+  </si>
+  <si>
+    <t>AGAS SINATRYA</t>
+  </si>
+  <si>
+    <t>85848380655</t>
+  </si>
+  <si>
+    <t>12020119130078</t>
+  </si>
+  <si>
+    <t>AHMAD SATRIA POLEM</t>
+  </si>
+  <si>
+    <t>81396636823</t>
   </si>
   <si>
     <t>Ekonomi</t>
   </si>
   <si>
-    <t>12030119140141</t>
-  </si>
-  <si>
-    <t>ADITYA ARYA ATMAJA</t>
-  </si>
-  <si>
-    <t>85156751464</t>
+    <t>12030119140159</t>
+  </si>
+  <si>
+    <t>AKRAM FAUZAN</t>
+  </si>
+  <si>
+    <t>82139484699</t>
   </si>
   <si>
     <t>Akuntansi</t>
   </si>
   <si>
-    <t>12030119140184</t>
-  </si>
-  <si>
-    <t>ACHMAD FAISAL YUNIANTO</t>
-  </si>
-  <si>
-    <t>8112906704</t>
-  </si>
-  <si>
-    <t>12030119140265</t>
-  </si>
-  <si>
-    <t>ADITYA WIRANANDA HIDAYAT</t>
-  </si>
-  <si>
-    <t>81218937418</t>
-  </si>
-  <si>
-    <t>13010119120019</t>
-  </si>
-  <si>
-    <t>Ananda Clarenita</t>
+    <t>13010118120046</t>
+  </si>
+  <si>
+    <t>agung tri suseno</t>
+  </si>
+  <si>
+    <t>8995796384</t>
+  </si>
+  <si>
+    <t>Sastra Indonesia</t>
+  </si>
+  <si>
+    <t>Fakultas Ilmu Budaya</t>
+  </si>
+  <si>
+    <t>13010118130104</t>
+  </si>
+  <si>
+    <t>Ahmad Multazam</t>
+  </si>
+  <si>
+    <t>85848177914</t>
+  </si>
+  <si>
+    <t>13010119120005</t>
+  </si>
+  <si>
+    <t>Anik Anggraini</t>
   </si>
   <si>
     <t>Perempuan</t>
   </si>
   <si>
-    <t>85700871836</t>
-  </si>
-  <si>
-    <t>Sastra Indonesia</t>
-  </si>
-  <si>
-    <t>Fakultas Ilmu Budaya</t>
-  </si>
-  <si>
-    <t>13010119130030</t>
-  </si>
-  <si>
-    <t>Almira Fadiah Rahma</t>
-  </si>
-  <si>
-    <t>89659602550</t>
-  </si>
-  <si>
-    <t>13010119130057</t>
-  </si>
-  <si>
-    <t>Aldilla Natasya Gunawan</t>
-  </si>
-  <si>
-    <t>87807546485</t>
-  </si>
-  <si>
-    <t>13010119140121</t>
-  </si>
-  <si>
-    <t>Amarel Aulia Zulfah</t>
-  </si>
-  <si>
-    <t>82220672788</t>
-  </si>
-  <si>
-    <t>13010119140134</t>
-  </si>
-  <si>
-    <t>Amalina Riyadlotul Kholisha</t>
-  </si>
-  <si>
-    <t>81326331472</t>
-  </si>
-  <si>
-    <t>13020218130049</t>
-  </si>
-  <si>
-    <t>ALVINA FARASINTA DEANTINA CHANDRA DEWI MALIK</t>
-  </si>
-  <si>
-    <t>81234712397</t>
+    <t>87730347297</t>
+  </si>
+  <si>
+    <t>13010119130027</t>
+  </si>
+  <si>
+    <t>ANNIDA SALSABILLAH</t>
+  </si>
+  <si>
+    <t>81292074588</t>
+  </si>
+  <si>
+    <t>13020217140023</t>
+  </si>
+  <si>
+    <t>ALDO JUAN ADITYA</t>
+  </si>
+  <si>
+    <t>85231624214</t>
   </si>
   <si>
     <t>Bahasa dan Kebudayaan Jepang</t>
   </si>
   <si>
-    <t>13020219130033</t>
-  </si>
-  <si>
-    <t>Aliyya Keumala Hayati Karebet</t>
-  </si>
-  <si>
-    <t>82245084521</t>
-  </si>
-  <si>
-    <t>13020219130040</t>
-  </si>
-  <si>
-    <t>Alya Nadya Putri Andika</t>
-  </si>
-  <si>
-    <t>895380903230</t>
-  </si>
-  <si>
-    <t>13020219130076</t>
-  </si>
-  <si>
-    <t>Adam aprylliano susakha</t>
-  </si>
-  <si>
-    <t>895384053446</t>
-  </si>
-  <si>
-    <t>13040119130056</t>
-  </si>
-  <si>
-    <t>Ananda Ihda Maulina</t>
-  </si>
-  <si>
-    <t>81326685778</t>
+    <t>13020219120016</t>
+  </si>
+  <si>
+    <t>Anggita Prameswari</t>
+  </si>
+  <si>
+    <t>83872888983</t>
+  </si>
+  <si>
+    <t>13020219120017</t>
+  </si>
+  <si>
+    <t>Annisa Nanda pradewi</t>
+  </si>
+  <si>
+    <t>81567612625</t>
+  </si>
+  <si>
+    <t>13020219130029</t>
+  </si>
+  <si>
+    <t>Anisa Aurelee Sudjarwoko</t>
+  </si>
+  <si>
+    <t>81291218303</t>
+  </si>
+  <si>
+    <t>13020219140105</t>
+  </si>
+  <si>
+    <t>AKMAL SYUHADA</t>
+  </si>
+  <si>
+    <t>82135591307</t>
+  </si>
+  <si>
+    <t>13020219140107</t>
+  </si>
+  <si>
+    <t>ANANDA NURUL FARAH</t>
+  </si>
+  <si>
+    <t>81211547173</t>
+  </si>
+  <si>
+    <t>13040119120003</t>
+  </si>
+  <si>
+    <t>Anjas Saputri Apriliana</t>
+  </si>
+  <si>
+    <t>85727263552</t>
   </si>
   <si>
     <t>Ilmu Perpustakaan</t>
   </si>
   <si>
-    <t>13040119140111</t>
-  </si>
-  <si>
-    <t>A Evan Harso Kristanto</t>
-  </si>
-  <si>
-    <t>81294360464</t>
-  </si>
-  <si>
-    <t>13040219120028</t>
-  </si>
-  <si>
-    <t>Abdur Rachman Fajri</t>
-  </si>
-  <si>
-    <t>87761721755</t>
+    <t>13040119130069</t>
+  </si>
+  <si>
+    <t>Anggie Yolanda</t>
+  </si>
+  <si>
+    <t>89506125521</t>
+  </si>
+  <si>
+    <t>13040119140125</t>
+  </si>
+  <si>
+    <t>Agus Sugiarto</t>
+  </si>
+  <si>
+    <t>87708738032</t>
+  </si>
+  <si>
+    <t>13040219130091</t>
+  </si>
+  <si>
+    <t>Anastasya</t>
+  </si>
+  <si>
+    <t>895335305772</t>
   </si>
   <si>
     <t>Antropologi Sosial</t>
   </si>
   <si>
-    <t>13040219130069</t>
-  </si>
-  <si>
-    <t>Abdan Syakoero</t>
-  </si>
-  <si>
-    <t>81293544999</t>
-  </si>
-  <si>
-    <t>13040219140121</t>
-  </si>
-  <si>
-    <t>Alysha Qotrun Nabila</t>
-  </si>
-  <si>
-    <t>85328907026</t>
-  </si>
-  <si>
-    <t>13040219140122</t>
-  </si>
-  <si>
-    <t>Achsin Kamal Faza</t>
-  </si>
-  <si>
-    <t>85727303148</t>
-  </si>
-  <si>
-    <t>21010119120007</t>
-  </si>
-  <si>
-    <t>Damaris Anggun Sasmita</t>
-  </si>
-  <si>
-    <t>89669536050</t>
+    <t>13040219140096</t>
+  </si>
+  <si>
+    <t>Anisa Indri Safitri</t>
+  </si>
+  <si>
+    <t>85742658821</t>
+  </si>
+  <si>
+    <t>21010119130094</t>
+  </si>
+  <si>
+    <t>Dian Laksita Adhitama</t>
+  </si>
+  <si>
+    <t>81228971878</t>
   </si>
   <si>
     <t>Teknik Sipil</t>
@@ -319,304 +310,301 @@
     <t>Fakultas Teknik</t>
   </si>
   <si>
-    <t>21010119120026</t>
-  </si>
-  <si>
-    <t>Feri Ardiansyah</t>
-  </si>
-  <si>
-    <t>895379169014</t>
-  </si>
-  <si>
-    <t>21010119120031</t>
-  </si>
-  <si>
-    <t>Clara Bella M</t>
-  </si>
-  <si>
-    <t>85372473051</t>
-  </si>
-  <si>
-    <t>21010119140161</t>
-  </si>
-  <si>
-    <t>Fathya Kautsar Rizkiananda</t>
-  </si>
-  <si>
-    <t>85900095941</t>
-  </si>
-  <si>
-    <t>21020119130126</t>
-  </si>
-  <si>
-    <t>Brigitta Edelweis Mekarwangi</t>
-  </si>
-  <si>
-    <t>81296153161</t>
+    <t>21020119130080</t>
+  </si>
+  <si>
+    <t>Dini Sriwahyuni</t>
+  </si>
+  <si>
+    <t>895361540564</t>
   </si>
   <si>
     <t>Arsitektur</t>
   </si>
   <si>
-    <t>21020119140130</t>
-  </si>
-  <si>
-    <t>Chintya Aulia Haninditha</t>
-  </si>
-  <si>
-    <t>81215782755</t>
-  </si>
-  <si>
-    <t>21020119140150</t>
-  </si>
-  <si>
-    <t>Fauzan Fathul Huda</t>
-  </si>
-  <si>
-    <t>85713170353</t>
-  </si>
-  <si>
-    <t>21020119140178</t>
-  </si>
-  <si>
-    <t>Deriana Salsa Puspa Kamila</t>
-  </si>
-  <si>
-    <t>85159700722</t>
-  </si>
-  <si>
-    <t>21030119130102</t>
-  </si>
-  <si>
-    <t>Carolina Wida Pertiwi</t>
-  </si>
-  <si>
-    <t>89608028218</t>
+    <t>21020119140154</t>
+  </si>
+  <si>
+    <t>Dinar Syaharani</t>
+  </si>
+  <si>
+    <t>81292277695</t>
+  </si>
+  <si>
+    <t>21020119140171</t>
+  </si>
+  <si>
+    <t>Dian Ayu Anggraini</t>
+  </si>
+  <si>
+    <t>81327276222</t>
+  </si>
+  <si>
+    <t>21020119140177</t>
+  </si>
+  <si>
+    <t>Dita Audina</t>
+  </si>
+  <si>
+    <t>81380656502</t>
+  </si>
+  <si>
+    <t>21030119120010</t>
+  </si>
+  <si>
+    <t>Dewi Atika Puji Astuti</t>
+  </si>
+  <si>
+    <t>81575866038</t>
   </si>
   <si>
     <t>Teknik Kimia</t>
   </si>
   <si>
-    <t>21030119190175</t>
-  </si>
-  <si>
-    <t>Brillian Talenta Berttyana</t>
-  </si>
-  <si>
-    <t>85159449064</t>
-  </si>
-  <si>
-    <t>21040119130068</t>
-  </si>
-  <si>
-    <t>Farrel Nabiel Melvinno</t>
-  </si>
-  <si>
-    <t>85741608608</t>
+    <t>21030119130121</t>
+  </si>
+  <si>
+    <t>Fransiskus Kevin</t>
+  </si>
+  <si>
+    <t>8981033372</t>
+  </si>
+  <si>
+    <t>21030119130123</t>
+  </si>
+  <si>
+    <t>George Elia Parlindungan</t>
+  </si>
+  <si>
+    <t>87871777902</t>
+  </si>
+  <si>
+    <t>21030119140164</t>
+  </si>
+  <si>
+    <t>Devina Karladisa Januria Syavaleda</t>
+  </si>
+  <si>
+    <t>85725057395</t>
+  </si>
+  <si>
+    <t>21040119120017</t>
+  </si>
+  <si>
+    <t>Dinda Aditya Noviana</t>
+  </si>
+  <si>
+    <t>82242628630</t>
   </si>
   <si>
     <t>Perencanaan Wilayah dan Kota</t>
   </si>
   <si>
-    <t>21070118130172</t>
-  </si>
-  <si>
-    <t>Fikrianuari Wibowo</t>
-  </si>
-  <si>
-    <t>89527941622</t>
-  </si>
-  <si>
-    <t>Teknik Industri</t>
-  </si>
-  <si>
-    <t>21090119130046</t>
-  </si>
-  <si>
-    <t>Febriyansyah Eko Ardhi Nugroho</t>
-  </si>
-  <si>
-    <t>82235669186</t>
+    <t>21040119130040</t>
+  </si>
+  <si>
+    <t>Galih Hafidzi Tahier</t>
+  </si>
+  <si>
+    <t>87873889057</t>
+  </si>
+  <si>
+    <t>21040119140162</t>
+  </si>
+  <si>
+    <t>Dinda Yunita Salsabila</t>
+  </si>
+  <si>
+    <t>89509020587</t>
+  </si>
+  <si>
+    <t>21040119140170</t>
+  </si>
+  <si>
+    <t>Gabriel Malvin Goklas</t>
+  </si>
+  <si>
+    <t>89636271395</t>
+  </si>
+  <si>
+    <t>21060119120029</t>
+  </si>
+  <si>
+    <t>Gabriel Haposan Siahaan</t>
+  </si>
+  <si>
+    <t>81257724175</t>
+  </si>
+  <si>
+    <t>Teknik Elektro</t>
+  </si>
+  <si>
+    <t>21060119130096</t>
+  </si>
+  <si>
+    <t>Ganang Aditya Pratama</t>
+  </si>
+  <si>
+    <t>8976206893</t>
+  </si>
+  <si>
+    <t>21060119130100</t>
+  </si>
+  <si>
+    <t>Filbert Hansel Purnomo</t>
+  </si>
+  <si>
+    <t>85156384370</t>
+  </si>
+  <si>
+    <t>21090119140143</t>
+  </si>
+  <si>
+    <t>Gamal Ikhsan Rasyid</t>
+  </si>
+  <si>
+    <t>81310851324</t>
   </si>
   <si>
     <t>Teknik Perkapalan</t>
   </si>
   <si>
-    <t>21100119120026</t>
-  </si>
-  <si>
-    <t>Defita Ayu Amalia</t>
-  </si>
-  <si>
-    <t>81901057270</t>
-  </si>
-  <si>
-    <t>Teknik Geologi</t>
-  </si>
-  <si>
-    <t>21110119120018</t>
-  </si>
-  <si>
-    <t>Channana Nadiya Salma</t>
-  </si>
-  <si>
-    <t>85875472045</t>
+    <t>21110119130064</t>
+  </si>
+  <si>
+    <t>Galih Annartiwang</t>
+  </si>
+  <si>
+    <t>89530232590</t>
   </si>
   <si>
     <t>Teknik Geodesi</t>
   </si>
   <si>
-    <t>21110119130049</t>
-  </si>
-  <si>
-    <t>Ferry Bakti Santoso</t>
-  </si>
-  <si>
-    <t>81317937412</t>
-  </si>
-  <si>
-    <t>21110119130084</t>
-  </si>
-  <si>
-    <t>Ferel Rico Albani</t>
-  </si>
-  <si>
-    <t>81295410973</t>
-  </si>
-  <si>
-    <t>21110119130111</t>
-  </si>
-  <si>
-    <t>Cynara Olivia Kusumacitra</t>
-  </si>
-  <si>
-    <t>85640805002</t>
-  </si>
-  <si>
-    <t>21120119120001</t>
-  </si>
-  <si>
-    <t>Fiki Rilo Pambudi</t>
-  </si>
-  <si>
-    <t>89670641830</t>
-  </si>
-  <si>
-    <t>Teknik Komputer</t>
-  </si>
-  <si>
-    <t>21120119140124</t>
-  </si>
-  <si>
-    <t>Fauzan Zaman</t>
-  </si>
-  <si>
-    <t>81291289944</t>
-  </si>
-  <si>
-    <t>22030119120008</t>
-  </si>
-  <si>
-    <t>Ni Putu Ari Trisma Damayanti</t>
-  </si>
-  <si>
-    <t>81246276642</t>
+    <t>21110119130069</t>
+  </si>
+  <si>
+    <t>Dinda Sifah Chanie Fahnevi</t>
+  </si>
+  <si>
+    <t>83871281364</t>
+  </si>
+  <si>
+    <t>21110119130104</t>
+  </si>
+  <si>
+    <t>Firdaus Mulya Wardhana</t>
+  </si>
+  <si>
+    <t>85848490763</t>
+  </si>
+  <si>
+    <t>22010317140045</t>
+  </si>
+  <si>
+    <t>NUR AGHNIA AZIZAH</t>
+  </si>
+  <si>
+    <t>81250040900</t>
+  </si>
+  <si>
+    <t>Farmasi</t>
+  </si>
+  <si>
+    <t>Fakultas Kedokteran</t>
+  </si>
+  <si>
+    <t>22030119100171</t>
+  </si>
+  <si>
+    <t>NURMARITA JAWI RIANTARI KAMBU</t>
+  </si>
+  <si>
+    <t>82395525892</t>
   </si>
   <si>
     <t>Gizi</t>
   </si>
   <si>
-    <t>Fakultas Kedokteran</t>
-  </si>
-  <si>
-    <t>22030119120011</t>
-  </si>
-  <si>
-    <t>Mita Ayu Lestari</t>
-  </si>
-  <si>
-    <t>85777285550</t>
-  </si>
-  <si>
-    <t>22030119120018</t>
-  </si>
-  <si>
-    <t>Nawati Auliatin</t>
-  </si>
-  <si>
-    <t>85336749927</t>
-  </si>
-  <si>
-    <t>22030119130047</t>
-  </si>
-  <si>
-    <t>Nadiya Mutiara</t>
-  </si>
-  <si>
-    <t>83815373264</t>
-  </si>
-  <si>
-    <t>22030119130056</t>
-  </si>
-  <si>
-    <t>Nourmalia Indah Prasanti</t>
-  </si>
-  <si>
-    <t>87889605883</t>
-  </si>
-  <si>
-    <t>22030119130088</t>
-  </si>
-  <si>
-    <t>Mutiara Putri Arasy</t>
-  </si>
-  <si>
-    <t>85931966455</t>
-  </si>
-  <si>
-    <t>22030119130090</t>
-  </si>
-  <si>
-    <t>Nikitasari Hilmia Rahma</t>
-  </si>
-  <si>
-    <t>82143201431</t>
-  </si>
-  <si>
-    <t>22030119140129</t>
-  </si>
-  <si>
-    <t>NIZA IANA TZANI</t>
-  </si>
-  <si>
-    <t>81228090010</t>
-  </si>
-  <si>
-    <t>22030119140132</t>
-  </si>
-  <si>
-    <t>NADIA BUDI PRATIWI</t>
-  </si>
-  <si>
-    <t>81211553915</t>
-  </si>
-  <si>
-    <t>22030119140143</t>
-  </si>
-  <si>
-    <t>NANDITA MAWA AYUNING PRAMESTI</t>
-  </si>
-  <si>
-    <t>82118607878</t>
-  </si>
-  <si>
-    <t>40011319650011</t>
-  </si>
-  <si>
-    <t>GALUH KUSDARMATUHENI UTAMI</t>
-  </si>
-  <si>
-    <t>85225980531</t>
+    <t>22030119120013</t>
+  </si>
+  <si>
+    <t>Olivia Ikhlas Prasasti</t>
+  </si>
+  <si>
+    <t>83824768107</t>
+  </si>
+  <si>
+    <t>22030119130060</t>
+  </si>
+  <si>
+    <t>Olivia Ruth Tio Yolanda Sibarani</t>
+  </si>
+  <si>
+    <t>89653415265</t>
+  </si>
+  <si>
+    <t>22030119130091</t>
+  </si>
+  <si>
+    <t>Olivia Luna Ariawan</t>
+  </si>
+  <si>
+    <t>81228040160</t>
+  </si>
+  <si>
+    <t>22030119130104</t>
+  </si>
+  <si>
+    <t>PUTRI AYU RAHMA PRATIWI</t>
+  </si>
+  <si>
+    <t>89670960016</t>
+  </si>
+  <si>
+    <t>22030119130112</t>
+  </si>
+  <si>
+    <t>Puspita Dian Pratiwi</t>
+  </si>
+  <si>
+    <t>89685855313</t>
+  </si>
+  <si>
+    <t>22030119140109</t>
+  </si>
+  <si>
+    <t>NUR BELLA TURCICA ANIBAH</t>
+  </si>
+  <si>
+    <t>82175715376</t>
+  </si>
+  <si>
+    <t>22030119140142</t>
+  </si>
+  <si>
+    <t>PASHARENA RISA SURYANINGRUM</t>
+  </si>
+  <si>
+    <t>82313216474</t>
+  </si>
+  <si>
+    <t>22030119140145</t>
+  </si>
+  <si>
+    <t>NYOMAN PUTRI ARI AMELINDA</t>
+  </si>
+  <si>
+    <t>82144853385</t>
+  </si>
+  <si>
+    <t>40011319650016</t>
+  </si>
+  <si>
+    <t>HUBBIBA NUR AN NISA</t>
+  </si>
+  <si>
+    <t>87786747350</t>
   </si>
   <si>
     <t>Manajemen dan Administrasi Logistik</t>
@@ -625,286 +613,286 @@
     <t>Sekolah Vokasi</t>
   </si>
   <si>
-    <t>40011319650028</t>
-  </si>
-  <si>
-    <t>FITRIA NUR ANGGRAINI</t>
-  </si>
-  <si>
-    <t>87831240071</t>
-  </si>
-  <si>
-    <t>40011319650046</t>
-  </si>
-  <si>
-    <t>FELIA NURUL HIDAYAT</t>
-  </si>
-  <si>
-    <t>85886643998</t>
-  </si>
-  <si>
-    <t>40011319650048</t>
-  </si>
-  <si>
-    <t>AHMAD DWINANDA ARIIJ TSAQIEV</t>
-  </si>
-  <si>
-    <t>89628113926</t>
-  </si>
-  <si>
-    <t>40011319650060</t>
-  </si>
-  <si>
-    <t>FARIDA NOVIANTI</t>
-  </si>
-  <si>
-    <t>85713320786</t>
-  </si>
-  <si>
-    <t>40011319650076</t>
-  </si>
-  <si>
-    <t>FYONA ADMALIZA BR BANGUN</t>
-  </si>
-  <si>
-    <t>83124663918</t>
-  </si>
-  <si>
-    <t>40011319650154</t>
-  </si>
-  <si>
-    <t>AHMAD DAFA BAHITS RIZQULLOH</t>
-  </si>
-  <si>
-    <t>82214275167</t>
-  </si>
-  <si>
-    <t>40011319650165</t>
-  </si>
-  <si>
-    <t>FELISSHA SAFA NAILA</t>
-  </si>
-  <si>
-    <t>81337593309</t>
-  </si>
-  <si>
-    <t>40011319650178</t>
-  </si>
-  <si>
-    <t>FEBRIAN INDAH KARTIKASARI</t>
-  </si>
-  <si>
-    <t>85161509020</t>
-  </si>
-  <si>
-    <t>40011319650184</t>
-  </si>
-  <si>
-    <t>ALAM TABAH PAMUJI</t>
-  </si>
-  <si>
-    <t>82220966707</t>
-  </si>
-  <si>
-    <t>40011419650015</t>
-  </si>
-  <si>
-    <t>GLADIS CHRIST BINTARI SAPTONO</t>
-  </si>
-  <si>
-    <t>81229350600</t>
+    <t>40011319650019</t>
+  </si>
+  <si>
+    <t>IMMA RIZKANUR FAJARWATI</t>
+  </si>
+  <si>
+    <t>81217694720</t>
+  </si>
+  <si>
+    <t>40011319650023</t>
+  </si>
+  <si>
+    <t>WICAKSONO ANDY KUNCORO</t>
+  </si>
+  <si>
+    <t>6289603531053</t>
+  </si>
+  <si>
+    <t>40011319650025</t>
+  </si>
+  <si>
+    <t>HANA RIZKYA AMALIA</t>
+  </si>
+  <si>
+    <t>85803347455</t>
+  </si>
+  <si>
+    <t>40011319650026</t>
+  </si>
+  <si>
+    <t>IMELDA HANGGARMUKTY</t>
+  </si>
+  <si>
+    <t>81388802454</t>
+  </si>
+  <si>
+    <t>40011319650045</t>
+  </si>
+  <si>
+    <t>ZENDA FATHUR RIFQI</t>
+  </si>
+  <si>
+    <t>89667909728</t>
+  </si>
+  <si>
+    <t>40011319650111</t>
+  </si>
+  <si>
+    <t>HASNA ATIKAH SALSABILA</t>
+  </si>
+  <si>
+    <t>85601213688</t>
+  </si>
+  <si>
+    <t>40011319650114</t>
+  </si>
+  <si>
+    <t>HELENA PUNKY RAHMAWATI</t>
+  </si>
+  <si>
+    <t>81326741612</t>
+  </si>
+  <si>
+    <t>40011319650140</t>
+  </si>
+  <si>
+    <t>YUDA AQIL SIRAJ</t>
+  </si>
+  <si>
+    <t>85377212000</t>
+  </si>
+  <si>
+    <t>40011319650169</t>
+  </si>
+  <si>
+    <t>ZESAR YUDHA PRIAMBODO</t>
+  </si>
+  <si>
+    <t>87760520904</t>
+  </si>
+  <si>
+    <t>40011319650177</t>
+  </si>
+  <si>
+    <t>HEPPY ANJANI</t>
+  </si>
+  <si>
+    <t>895421843217</t>
+  </si>
+  <si>
+    <t>40011419650023</t>
+  </si>
+  <si>
+    <t>HANAN HAURA YUZAN</t>
+  </si>
+  <si>
+    <t>82279434984</t>
   </si>
   <si>
     <t>Akuntansi Perpajakan</t>
   </si>
   <si>
-    <t>40011419650048</t>
-  </si>
-  <si>
-    <t>Fathyn Fadhillah Yunda</t>
-  </si>
-  <si>
-    <t>81270681912</t>
-  </si>
-  <si>
-    <t>40011419650091</t>
-  </si>
-  <si>
-    <t>HAMMALKA TARAZU PRAMUDYAWARDHANI</t>
-  </si>
-  <si>
-    <t>81222012021</t>
-  </si>
-  <si>
-    <t>40011419650153</t>
-  </si>
-  <si>
-    <t>FRISKA DEANOVA</t>
-  </si>
-  <si>
-    <t>85938353050</t>
-  </si>
-  <si>
-    <t>40011419650194</t>
-  </si>
-  <si>
-    <t>GITARETA AMARANGGANA ARYANA HIDAYAT</t>
-  </si>
-  <si>
-    <t>85828830973</t>
-  </si>
-  <si>
-    <t>40011419650224</t>
-  </si>
-  <si>
-    <t>FINA KAMILA PUTRI</t>
-  </si>
-  <si>
-    <t>85640040189</t>
-  </si>
-  <si>
-    <t>40011419650260</t>
-  </si>
-  <si>
-    <t>GRACE AMELIA NURUL ADHA</t>
-  </si>
-  <si>
-    <t>89618697734</t>
-  </si>
-  <si>
-    <t>40011419650325</t>
-  </si>
-  <si>
-    <t>FORTUNELLA FARLYAGIZA</t>
-  </si>
-  <si>
-    <t>89672702374</t>
-  </si>
-  <si>
-    <t>40020519650027</t>
-  </si>
-  <si>
-    <t>FRANSISKA AULIA FITRIYANI</t>
-  </si>
-  <si>
-    <t>81390060904</t>
-  </si>
-  <si>
-    <t>Bahasa Asing Terapan</t>
-  </si>
-  <si>
-    <t>40020519650043</t>
-  </si>
-  <si>
-    <t>FATIYA MUTSAQQOFA</t>
-  </si>
-  <si>
-    <t>895392326507</t>
-  </si>
-  <si>
-    <t>40020519650068</t>
-  </si>
-  <si>
-    <t>FRULLY ZULFANIA ARRAHMA</t>
-  </si>
-  <si>
-    <t>81226503259</t>
-  </si>
-  <si>
-    <t>40030519650010</t>
-  </si>
-  <si>
-    <t>Ahmed Rizki Habibie</t>
-  </si>
-  <si>
-    <t>81210058772</t>
+    <t>40011419650029</t>
+  </si>
+  <si>
+    <t>IKTIA AMILINA SARI</t>
+  </si>
+  <si>
+    <t>81237691123</t>
+  </si>
+  <si>
+    <t>40011419650082</t>
+  </si>
+  <si>
+    <t>WAHYUDIN IHSAN ALAMIN</t>
+  </si>
+  <si>
+    <t>81268490498</t>
+  </si>
+  <si>
+    <t>40011419650086</t>
+  </si>
+  <si>
+    <t>Ichvari Aisyah Melinia</t>
+  </si>
+  <si>
+    <t>85966177040</t>
+  </si>
+  <si>
+    <t>40011419650121</t>
+  </si>
+  <si>
+    <t>YOGIE NOORPRASETYA</t>
+  </si>
+  <si>
+    <t>82220528422</t>
+  </si>
+  <si>
+    <t>40011419650190</t>
+  </si>
+  <si>
+    <t>IMELDA HELDIYANI MUZIZAH</t>
+  </si>
+  <si>
+    <t>82322277303</t>
+  </si>
+  <si>
+    <t>40011419650241</t>
+  </si>
+  <si>
+    <t>HOFIFAH ZAETUN SIDDIQ</t>
+  </si>
+  <si>
+    <t>85210723252</t>
+  </si>
+  <si>
+    <t>40011419650286</t>
+  </si>
+  <si>
+    <t>IDA NOVISAH</t>
+  </si>
+  <si>
+    <t>85860380112</t>
+  </si>
+  <si>
+    <t>40011419650326</t>
+  </si>
+  <si>
+    <t>ZHUDA ASSIDIQ</t>
+  </si>
+  <si>
+    <t>81329205836</t>
+  </si>
+  <si>
+    <t>40011419650342</t>
+  </si>
+  <si>
+    <t>HANIFAH ZAFIRA</t>
+  </si>
+  <si>
+    <t>81374543095</t>
+  </si>
+  <si>
+    <t>40030519650107</t>
+  </si>
+  <si>
+    <t>Higha Vista</t>
+  </si>
+  <si>
+    <t>81809757207</t>
   </si>
   <si>
     <t>Teknik Infrastruktur Sipil dan Perancangan Arsitek</t>
   </si>
   <si>
-    <t>40030619650050</t>
-  </si>
-  <si>
-    <t>FORINA YOSYTA RIZKY</t>
-  </si>
-  <si>
-    <t>81226519095</t>
+    <t>40030519650125</t>
+  </si>
+  <si>
+    <t>Yitzak Kamya Leiwakabessy</t>
+  </si>
+  <si>
+    <t>81919990412</t>
+  </si>
+  <si>
+    <t>40030619650024</t>
+  </si>
+  <si>
+    <t>HASNA JAUHARAH LESMANA</t>
+  </si>
+  <si>
+    <t>81219692684</t>
   </si>
   <si>
     <t>Perencanaan Tata Ruang dan Pertanahan</t>
   </si>
   <si>
-    <t>40040219650010</t>
-  </si>
-  <si>
-    <t>AGADE BANDULE</t>
-  </si>
-  <si>
-    <t>89636806055</t>
+    <t>40030619650048</t>
+  </si>
+  <si>
+    <t>HASTI NOVITA SARI</t>
+  </si>
+  <si>
+    <t>89525647907</t>
+  </si>
+  <si>
+    <t>40030619650066</t>
+  </si>
+  <si>
+    <t>HANIFAH NUR RIFDAH SAVITRI</t>
+  </si>
+  <si>
+    <t>82110221100</t>
+  </si>
+  <si>
+    <t>40030619650124</t>
+  </si>
+  <si>
+    <t>INASA RIFDATUL IZZATI LILLAH</t>
+  </si>
+  <si>
+    <t>82223727335</t>
+  </si>
+  <si>
+    <t>40040219650086</t>
+  </si>
+  <si>
+    <t>ZUHDAN ROSIDI</t>
+  </si>
+  <si>
+    <t>81314422575</t>
   </si>
   <si>
     <t>Rekayasa Perancangan Mekanik</t>
   </si>
   <si>
-    <t>40040219650011</t>
-  </si>
-  <si>
-    <t>AHMAD RUSDIYANTO</t>
-  </si>
-  <si>
-    <t>81217040810</t>
-  </si>
-  <si>
-    <t>40040219650077</t>
-  </si>
-  <si>
-    <t>AGUS CATUROKHMAN</t>
-  </si>
-  <si>
-    <t>85727557003</t>
-  </si>
-  <si>
-    <t>40040219650089</t>
-  </si>
-  <si>
-    <t>AGHI HENDRAWAN</t>
-  </si>
-  <si>
-    <t>85231227416</t>
-  </si>
-  <si>
-    <t>40040219650107</t>
-  </si>
-  <si>
-    <t>AGA HERNANDA</t>
-  </si>
-  <si>
-    <t>895603389504</t>
-  </si>
-  <si>
-    <t>40040319650049</t>
-  </si>
-  <si>
-    <t>FATIMAH AZ ZAHRA ZUKRA</t>
-  </si>
-  <si>
-    <t>81266137630</t>
-  </si>
-  <si>
-    <t>Teknologi Rekayasa Otomasi</t>
-  </si>
-  <si>
-    <t>40040419650029</t>
-  </si>
-  <si>
-    <t>AHMAD NAUFAL UMAR ATHALLAH</t>
-  </si>
-  <si>
-    <t>81387308493</t>
+    <t>40040419650018</t>
+  </si>
+  <si>
+    <t>YOGA RONI PRASETYO</t>
+  </si>
+  <si>
+    <t>85877706265</t>
   </si>
   <si>
     <t>Teknologi Rekayasa Konstruksi Perkapalan</t>
+  </si>
+  <si>
+    <t>14040119140128</t>
+  </si>
+  <si>
+    <t>STEPHANIE ALBERTINA IVANNA RAHAYAAN</t>
+  </si>
+  <si>
+    <t>087731071609</t>
+  </si>
+  <si>
+    <t>Ilmu Komunikasi</t>
+  </si>
+  <si>
+    <t>Fakultas Ilmu Sosial dan Ilmu Politik</t>
   </si>
 </sst>
 </file>
@@ -1720,7 +1708,7 @@
         <v>33</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>30</v>
@@ -1754,19 +1742,19 @@
         <v>3</v>
       </c>
       <c r="B10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>36</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>37</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>38</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>30</v>
@@ -1800,19 +1788,19 @@
         <v>4</v>
       </c>
       <c r="B11" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>40</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>38</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>30</v>
@@ -1858,10 +1846,10 @@
         <v>44</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
@@ -1892,22 +1880,22 @@
         <v>6</v>
       </c>
       <c r="B13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="G13" s="15" t="s">
         <v>46</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>50</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
@@ -1938,22 +1926,22 @@
         <v>7</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="15" t="s">
         <v>52</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>47</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>53</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
@@ -1990,16 +1978,16 @@
         <v>55</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>56</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
@@ -2036,16 +2024,16 @@
         <v>58</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>59</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
@@ -2076,22 +2064,22 @@
         <v>10</v>
       </c>
       <c r="B17" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>49</v>
-      </c>
       <c r="G17" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
@@ -2122,22 +2110,22 @@
         <v>11</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
@@ -2174,16 +2162,16 @@
         <v>68</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
@@ -2220,16 +2208,16 @@
         <v>71</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>72</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
@@ -2266,16 +2254,16 @@
         <v>74</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>75</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
@@ -2312,7 +2300,7 @@
         <v>77</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>78</v>
@@ -2321,7 +2309,7 @@
         <v>79</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
@@ -2358,7 +2346,7 @@
         <v>81</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>82</v>
@@ -2367,7 +2355,7 @@
         <v>79</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
@@ -2410,10 +2398,10 @@
         <v>85</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
@@ -2444,22 +2432,22 @@
         <v>18</v>
       </c>
       <c r="B25" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="D25" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="15" t="s">
+      <c r="F25" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F25" s="15" t="s">
-        <v>86</v>
-      </c>
       <c r="G25" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
@@ -2496,16 +2484,16 @@
         <v>91</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>92</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
@@ -2542,16 +2530,16 @@
         <v>94</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>95</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
@@ -2582,22 +2570,22 @@
         <v>21</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C28" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G28" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>100</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="16"/>
@@ -2628,22 +2616,22 @@
         <v>22</v>
       </c>
       <c r="B29" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>99</v>
-      </c>
       <c r="G29" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H29" s="16"/>
       <c r="I29" s="16"/>
@@ -2674,22 +2662,22 @@
         <v>23</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
@@ -2720,22 +2708,22 @@
         <v>24</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H31" s="16"/>
       <c r="I31" s="16"/>
@@ -2766,22 +2754,22 @@
         <v>25</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H32" s="16"/>
       <c r="I32" s="16"/>
@@ -2812,22 +2800,22 @@
         <v>26</v>
       </c>
       <c r="B33" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F33" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C33" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>113</v>
-      </c>
       <c r="G33" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H33" s="16"/>
       <c r="I33" s="16"/>
@@ -2858,22 +2846,22 @@
         <v>27</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>27</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H34" s="16"/>
       <c r="I34" s="16"/>
@@ -2904,22 +2892,22 @@
         <v>28</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H35" s="16"/>
       <c r="I35" s="16"/>
@@ -2950,22 +2938,22 @@
         <v>29</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H36" s="16"/>
       <c r="I36" s="16"/>
@@ -2996,22 +2984,22 @@
         <v>30</v>
       </c>
       <c r="B37" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="F37" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>126</v>
-      </c>
       <c r="G37" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H37" s="16"/>
       <c r="I37" s="16"/>
@@ -3042,22 +3030,22 @@
         <v>31</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H38" s="16"/>
       <c r="I38" s="16"/>
@@ -3100,10 +3088,10 @@
         <v>136</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H39" s="16"/>
       <c r="I39" s="16"/>
@@ -3134,22 +3122,22 @@
         <v>33</v>
       </c>
       <c r="B40" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" s="15" t="s">
         <v>138</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>139</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>27</v>
       </c>
       <c r="E40" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F40" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="F40" s="15" t="s">
-        <v>141</v>
-      </c>
       <c r="G40" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H40" s="16"/>
       <c r="I40" s="16"/>
@@ -3180,22 +3168,22 @@
         <v>34</v>
       </c>
       <c r="B41" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="D41" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D41" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>144</v>
-      </c>
       <c r="F41" s="15" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H41" s="16"/>
       <c r="I41" s="16"/>
@@ -3226,22 +3214,22 @@
         <v>35</v>
       </c>
       <c r="B42" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C42" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>148</v>
-      </c>
       <c r="F42" s="15" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H42" s="16"/>
       <c r="I42" s="16"/>
@@ -3272,22 +3260,22 @@
         <v>36</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>27</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H43" s="16"/>
       <c r="I43" s="16"/>
@@ -3318,22 +3306,22 @@
         <v>37</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>27</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H44" s="16"/>
       <c r="I44" s="16"/>
@@ -3364,22 +3352,22 @@
         <v>38</v>
       </c>
       <c r="B45" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C45" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="D45" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="D45" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>158</v>
-      </c>
       <c r="F45" s="15" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H45" s="16"/>
       <c r="I45" s="16"/>
@@ -3410,22 +3398,22 @@
         <v>39</v>
       </c>
       <c r="B46" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" s="15" t="s">
         <v>159</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>160</v>
       </c>
       <c r="D46" s="15" t="s">
         <v>27</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H46" s="16"/>
       <c r="I46" s="16"/>
@@ -3456,22 +3444,22 @@
         <v>40</v>
       </c>
       <c r="B47" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E47" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="F47" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="D47" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E47" s="15" t="s">
+      <c r="G47" s="15" t="s">
         <v>165</v>
-      </c>
-      <c r="F47" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="G47" s="15" t="s">
-        <v>100</v>
       </c>
       <c r="H47" s="16"/>
       <c r="I47" s="16"/>
@@ -3508,7 +3496,7 @@
         <v>167</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E48" s="15" t="s">
         <v>168</v>
@@ -3517,7 +3505,7 @@
         <v>169</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H48" s="16"/>
       <c r="I48" s="16"/>
@@ -3548,22 +3536,22 @@
         <v>42</v>
       </c>
       <c r="B49" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C49" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="D49" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="15" t="s">
         <v>172</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>173</v>
       </c>
       <c r="F49" s="15" t="s">
         <v>169</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H49" s="16"/>
       <c r="I49" s="16"/>
@@ -3594,22 +3582,22 @@
         <v>43</v>
       </c>
       <c r="B50" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C50" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="D50" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" s="15" t="s">
         <v>175</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>176</v>
       </c>
       <c r="F50" s="15" t="s">
         <v>169</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H50" s="16"/>
       <c r="I50" s="16"/>
@@ -3640,22 +3628,22 @@
         <v>44</v>
       </c>
       <c r="B51" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C51" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="D51" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E51" s="15" t="s">
         <v>178</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>179</v>
       </c>
       <c r="F51" s="15" t="s">
         <v>169</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H51" s="16"/>
       <c r="I51" s="16"/>
@@ -3686,22 +3674,22 @@
         <v>45</v>
       </c>
       <c r="B52" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="D52" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E52" s="15" t="s">
         <v>181</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>182</v>
       </c>
       <c r="F52" s="15" t="s">
         <v>169</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H52" s="16"/>
       <c r="I52" s="16"/>
@@ -3732,22 +3720,22 @@
         <v>46</v>
       </c>
       <c r="B53" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C53" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="D53" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>184</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>185</v>
       </c>
       <c r="F53" s="15" t="s">
         <v>169</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H53" s="16"/>
       <c r="I53" s="16"/>
@@ -3778,22 +3766,22 @@
         <v>47</v>
       </c>
       <c r="B54" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="D54" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E54" s="15" t="s">
         <v>187</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>188</v>
       </c>
       <c r="F54" s="15" t="s">
         <v>169</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H54" s="16"/>
       <c r="I54" s="16"/>
@@ -3824,22 +3812,22 @@
         <v>48</v>
       </c>
       <c r="B55" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C55" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="D55" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E55" s="15" t="s">
         <v>190</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>191</v>
       </c>
       <c r="F55" s="15" t="s">
         <v>169</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H55" s="16"/>
       <c r="I55" s="16"/>
@@ -3870,22 +3858,22 @@
         <v>49</v>
       </c>
       <c r="B56" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C56" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="C56" s="15" t="s">
+      <c r="D56" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E56" s="15" t="s">
         <v>193</v>
-      </c>
-      <c r="D56" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>194</v>
       </c>
       <c r="F56" s="15" t="s">
         <v>169</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H56" s="16"/>
       <c r="I56" s="16"/>
@@ -3916,22 +3904,22 @@
         <v>50</v>
       </c>
       <c r="B57" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="D57" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="D57" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E57" s="15" t="s">
+      <c r="F57" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="F57" s="15" t="s">
-        <v>169</v>
-      </c>
       <c r="G57" s="15" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="H57" s="16"/>
       <c r="I57" s="16"/>
@@ -3962,22 +3950,22 @@
         <v>51</v>
       </c>
       <c r="B58" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="G58" s="15" t="s">
         <v>198</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="D58" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="F58" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="G58" s="15" t="s">
-        <v>202</v>
       </c>
       <c r="H58" s="16"/>
       <c r="I58" s="16"/>
@@ -4008,22 +3996,22 @@
         <v>52</v>
       </c>
       <c r="B59" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C59" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="D59" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="D59" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>205</v>
-      </c>
       <c r="F59" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H59" s="16"/>
       <c r="I59" s="16"/>
@@ -4054,22 +4042,22 @@
         <v>53</v>
       </c>
       <c r="B60" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C60" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="D60" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E60" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="D60" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>208</v>
-      </c>
       <c r="F60" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H60" s="16"/>
       <c r="I60" s="16"/>
@@ -4100,22 +4088,22 @@
         <v>54</v>
       </c>
       <c r="B61" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C61" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="D61" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E61" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="D61" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>211</v>
-      </c>
       <c r="F61" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H61" s="16"/>
       <c r="I61" s="16"/>
@@ -4146,22 +4134,22 @@
         <v>55</v>
       </c>
       <c r="B62" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C62" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="D62" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="D62" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>214</v>
-      </c>
       <c r="F62" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H62" s="16"/>
       <c r="I62" s="16"/>
@@ -4192,22 +4180,22 @@
         <v>56</v>
       </c>
       <c r="B63" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="C63" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="C63" s="15" t="s">
+      <c r="D63" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E63" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="D63" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E63" s="15" t="s">
-        <v>217</v>
-      </c>
       <c r="F63" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H63" s="16"/>
       <c r="I63" s="16"/>
@@ -4238,22 +4226,22 @@
         <v>57</v>
       </c>
       <c r="B64" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C64" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="C64" s="15" t="s">
+      <c r="D64" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="D64" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>220</v>
-      </c>
       <c r="F64" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G64" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H64" s="16"/>
       <c r="I64" s="16"/>
@@ -4284,22 +4272,22 @@
         <v>58</v>
       </c>
       <c r="B65" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C65" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="C65" s="15" t="s">
+      <c r="D65" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="D65" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E65" s="15" t="s">
-        <v>223</v>
-      </c>
       <c r="F65" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H65" s="16"/>
       <c r="I65" s="16"/>
@@ -4330,22 +4318,22 @@
         <v>59</v>
       </c>
       <c r="B66" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="C66" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="C66" s="15" t="s">
+      <c r="D66" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E66" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="D66" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E66" s="15" t="s">
-        <v>226</v>
-      </c>
       <c r="F66" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G66" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H66" s="16"/>
       <c r="I66" s="16"/>
@@ -4376,22 +4364,22 @@
         <v>60</v>
       </c>
       <c r="B67" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C67" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="C67" s="15" t="s">
+      <c r="D67" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E67" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="D67" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E67" s="15" t="s">
-        <v>229</v>
-      </c>
       <c r="F67" s="15" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H67" s="16"/>
       <c r="I67" s="16"/>
@@ -4422,22 +4410,22 @@
         <v>61</v>
       </c>
       <c r="B68" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C68" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="C68" s="15" t="s">
+      <c r="D68" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E68" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="D68" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E68" s="15" t="s">
+      <c r="F68" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="F68" s="15" t="s">
-        <v>233</v>
-      </c>
       <c r="G68" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H68" s="16"/>
       <c r="I68" s="16"/>
@@ -4468,22 +4456,22 @@
         <v>62</v>
       </c>
       <c r="B69" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C69" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="D69" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E69" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="D69" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E69" s="15" t="s">
-        <v>236</v>
-      </c>
       <c r="F69" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H69" s="16"/>
       <c r="I69" s="16"/>
@@ -4514,22 +4502,22 @@
         <v>63</v>
       </c>
       <c r="B70" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="C70" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="C70" s="15" t="s">
+      <c r="D70" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E70" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="D70" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E70" s="15" t="s">
-        <v>239</v>
-      </c>
       <c r="F70" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G70" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H70" s="16"/>
       <c r="I70" s="16"/>
@@ -4560,22 +4548,22 @@
         <v>64</v>
       </c>
       <c r="B71" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C71" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="D71" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E71" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="D71" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E71" s="15" t="s">
-        <v>242</v>
-      </c>
       <c r="F71" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H71" s="16"/>
       <c r="I71" s="16"/>
@@ -4606,22 +4594,22 @@
         <v>65</v>
       </c>
       <c r="B72" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="C72" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="C72" s="15" t="s">
+      <c r="D72" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="D72" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E72" s="15" t="s">
-        <v>245</v>
-      </c>
       <c r="F72" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H72" s="16"/>
       <c r="I72" s="16"/>
@@ -4652,22 +4640,22 @@
         <v>66</v>
       </c>
       <c r="B73" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="C73" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="C73" s="15" t="s">
+      <c r="D73" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E73" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="D73" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E73" s="15" t="s">
-        <v>248</v>
-      </c>
       <c r="F73" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H73" s="16"/>
       <c r="I73" s="16"/>
@@ -4698,22 +4686,22 @@
         <v>67</v>
       </c>
       <c r="B74" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="C74" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="C74" s="15" t="s">
+      <c r="D74" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E74" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="D74" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E74" s="15" t="s">
-        <v>251</v>
-      </c>
       <c r="F74" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H74" s="16"/>
       <c r="I74" s="16"/>
@@ -4744,22 +4732,22 @@
         <v>68</v>
       </c>
       <c r="B75" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C75" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="C75" s="15" t="s">
+      <c r="D75" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E75" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="D75" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E75" s="15" t="s">
-        <v>254</v>
-      </c>
       <c r="F75" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H75" s="16"/>
       <c r="I75" s="16"/>
@@ -4790,22 +4778,22 @@
         <v>69</v>
       </c>
       <c r="B76" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="C76" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="C76" s="15" t="s">
+      <c r="D76" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E76" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="D76" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E76" s="15" t="s">
-        <v>257</v>
-      </c>
       <c r="F76" s="15" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="G76" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H76" s="16"/>
       <c r="I76" s="16"/>
@@ -4836,22 +4824,22 @@
         <v>70</v>
       </c>
       <c r="B77" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E77" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="C77" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="D77" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E77" s="15" t="s">
-        <v>261</v>
-      </c>
       <c r="F77" s="15" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="G77" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H77" s="16"/>
       <c r="I77" s="16"/>
@@ -4882,22 +4870,22 @@
         <v>71</v>
       </c>
       <c r="B78" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E78" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="C78" s="15" t="s">
+      <c r="F78" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="D78" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E78" s="15" t="s">
-        <v>264</v>
-      </c>
-      <c r="F78" s="15" t="s">
-        <v>258</v>
-      </c>
       <c r="G78" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H78" s="16"/>
       <c r="I78" s="16"/>
@@ -4928,22 +4916,22 @@
         <v>72</v>
       </c>
       <c r="B79" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="C79" s="15" t="s">
         <v>265</v>
-      </c>
-      <c r="C79" s="15" t="s">
-        <v>266</v>
       </c>
       <c r="D79" s="15" t="s">
         <v>27</v>
       </c>
       <c r="E79" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F79" s="15" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H79" s="16"/>
       <c r="I79" s="16"/>
@@ -4974,22 +4962,22 @@
         <v>73</v>
       </c>
       <c r="B80" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E80" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="C80" s="15" t="s">
+      <c r="F80" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="D80" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E80" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="F80" s="15" t="s">
-        <v>272</v>
-      </c>
       <c r="G80" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H80" s="16"/>
       <c r="I80" s="16"/>
@@ -5020,22 +5008,22 @@
         <v>74</v>
       </c>
       <c r="B81" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E81" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="C81" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="D81" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E81" s="15" t="s">
-        <v>275</v>
-      </c>
       <c r="F81" s="15" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G81" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H81" s="16"/>
       <c r="I81" s="16"/>
@@ -5066,22 +5054,22 @@
         <v>75</v>
       </c>
       <c r="B82" s="15" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D82" s="15" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E82" s="15" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F82" s="15" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G82" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H82" s="16"/>
       <c r="I82" s="16"/>
@@ -5112,22 +5100,22 @@
         <v>76</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D83" s="15" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E83" s="15" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F83" s="15" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G83" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H83" s="16"/>
       <c r="I83" s="16"/>
@@ -5158,22 +5146,22 @@
         <v>77</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D84" s="15" t="s">
         <v>27</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F84" s="15" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="G84" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H84" s="16"/>
       <c r="I84" s="16"/>
@@ -5204,22 +5192,22 @@
         <v>78</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D85" s="15" t="s">
         <v>27</v>
       </c>
       <c r="E85" s="15" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F85" s="15" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="G85" s="15" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H85" s="16"/>
       <c r="I85" s="16"/>
@@ -5250,22 +5238,22 @@
         <v>79</v>
       </c>
       <c r="B86" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="C86" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="C86" s="15" t="s">
+      <c r="D86" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E86" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="D86" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E86" s="15" t="s">
+      <c r="F86" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="F86" s="15" t="s">
+      <c r="G86" s="15" t="s">
         <v>292</v>
-      </c>
-      <c r="G86" s="15" t="s">
-        <v>202</v>
       </c>
       <c r="H86" s="16"/>
       <c r="I86" s="16"/>
@@ -5291,51 +5279,8 @@
         <f>IF(S86&gt;=80, "A", IF(S86&gt;=70, "B", IF(S86&gt;=60,"C",IF(S86&gt;=50, "D", "E"))))</f>
       </c>
     </row>
-    <row r="87" ht="24" customHeight="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A87" s="15">
-        <v>80</v>
-      </c>
-      <c r="B87" s="15" t="s">
-        <v>293</v>
-      </c>
-      <c r="C87" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="D87" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E87" s="15" t="s">
-        <v>295</v>
-      </c>
-      <c r="F87" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="G87" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="H87" s="16"/>
-      <c r="I87" s="16"/>
-      <c r="J87" s="16"/>
-      <c r="K87" s="16"/>
-      <c r="L87" s="16"/>
-      <c r="M87" s="16"/>
-      <c r="N87" s="16"/>
-      <c r="O87" s="16"/>
-      <c r="P87" s="17">
-        <f>((H87+I87+J87+L87+M87)/5)</f>
-      </c>
-      <c r="Q87" s="17">
-        <f>(K87+N87)/2</f>
-      </c>
-      <c r="R87" s="17">
-        <f>O87</f>
-      </c>
-      <c r="S87" s="17">
-        <f>((P87*50%)+(Q87*25%)+(R87*25%))</f>
-      </c>
-      <c r="T87" s="17">
-        <f>IF(S87&gt;=80, "A", IF(S87&gt;=70, "B", IF(S87&gt;=60,"C",IF(S87&gt;=50, "D", "E"))))</f>
-      </c>
+    <row r="87" ht="24" customHeight="1" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T87" s="18"/>
     </row>
     <row r="88" ht="24" customHeight="1" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T88" s="18"/>

</xml_diff>